<commit_message>
feat(export,ui): printable exports + totals; landscape PDF; UX/loading
- CSV/XLSX: make printable on short paper; auto-fit column widths
- CSV/XLSX: add TOTAL rows (per section and grand total); default blanks to 0
- PDF: implement generation; landscape orientation; long pages; include TOTAL in Per Barangay
- Formatting: DISASTER names rendered in ALL CAPS
- UX: generate CSV/XLSX without page reload or new tab
- UX: add robust loading states on pages and buttons; disable during work
- UI: beautify/refresh navbar styles and active states
- Dev note: add comment documenting dev_user id = 2 usage
- Verification: exercised with large datasets to validate layout and totals

chore(deps): install exceljs and puppeteer
</commit_message>
<xml_diff>
--- a/server/templates/Aggregated.xlsx
+++ b/server/templates/Aggregated.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\_VicenteBercasioII\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\_VicenteBercasioII\Documents\Github Projects\e-LegTas\server\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699BAB98-9CFD-40E7-B415-7266F3C6AA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C7CDF3-E309-41DB-92AB-975FED495651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{72FF522A-0EE4-40AE-8972-20260110F40D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -182,11 +181,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -650,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C70A77-9BA4-454C-941D-2E52BB0F8BDA}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,437 +662,1022 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="2" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="3"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="3"/>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="3"/>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="3"/>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3"/>
+      <c r="G109" s="3"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="3"/>
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1117,19 +1698,4 @@
   <pageSetup paperSize="10000" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD90E97F-295A-4742-8F26-F7B3347D63C9}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>